<commit_message>
updated DVM rules to include missing leg data sets updated data model to include leg data sets updated DVM test cases to include missing leg data sets consolidated the load_data_set_info.sql into load_ref_data.sql
</commit_message>
<xml_diff>
--- a/docs/QC Validation Criteria.xlsx
+++ b/docs/QC Validation Criteria.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse.Abdul\Documents\Version Control\Git\centralized-cruise-database\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse.abdul\Documents\Version Control\Git\centralized-cruise-database\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="116">
   <si>
     <t>WARN</t>
   </si>
@@ -514,6 +514,18 @@
   </si>
   <si>
     <t>(Category 3, 6, 7) Test Cases for overlapping data streams</t>
+  </si>
+  <si>
+    <t>MISS_DATA_SET_YN</t>
+  </si>
+  <si>
+    <t>Missing Leg Data Set</t>
+  </si>
+  <si>
+    <t>The Leg does not have any data sets defined for it</t>
+  </si>
+  <si>
+    <t>The Cruise ([CRUISE_NAME]) has a Cruise Leg ([LEG_NAME]) on the Vessel ([VESSEL_NAME]) with a Start Date ([FORMAT_LEG_START_DATE]) and End Date ([FORMAT_LEG_END_DATE]) that does not have at least one data set associated with it</t>
   </si>
 </sst>
 </file>
@@ -1020,8 +1032,8 @@
   <dimension ref="A1:X888"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1184,7 +1196,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4" t="str">
-        <f t="shared" ref="N3:N18" si="0">CONCATENATE("INSERT INTO DVM_ISS_TYPES (ISS_TYPE_NAME, ISS_TYPE_COMMENT_TEMPLATE, QC_OBJECT_ID, IND_FIELD_NAME, ISS_SEVERITY_ID, DATA_STREAM_ID, ISS_TYPE_ACTIVE_YN, ISS_TYPE_DESC, APP_LINK_TEMPLATE) VALUES ('", SUBSTITUTE(H3, "'", "''"), "', '", SUBSTITUTE(J3, "'", "''"), "', (SELECT QC_OBJECT_ID FROM DVM_QC_OBJECTS WHERE OBJECT_NAME = '", E3, "'), '", G3, "', (SELECT ISS_SEVERITY_ID FROM DVM_ISS_SEVERITY WHERE ISS_SEVERITY_CODE = '",D3, "'), (SELECT data_stream_id from DVM_data_streams where data_stream_code = '",A3, "'), 'Y', '", SUBSTITUTE(I3, "'", "''"), "', '", SUBSTITUTE(K3, "'", "''"), "');")</f>
+        <f t="shared" ref="N3:N19" si="0">CONCATENATE("INSERT INTO DVM_ISS_TYPES (ISS_TYPE_NAME, ISS_TYPE_COMMENT_TEMPLATE, QC_OBJECT_ID, IND_FIELD_NAME, ISS_SEVERITY_ID, DATA_STREAM_ID, ISS_TYPE_ACTIVE_YN, ISS_TYPE_DESC, APP_LINK_TEMPLATE) VALUES ('", SUBSTITUTE(H3, "'", "''"), "', '", SUBSTITUTE(J3, "'", "''"), "', (SELECT QC_OBJECT_ID FROM DVM_QC_OBJECTS WHERE OBJECT_NAME = '", E3, "'), '", G3, "', (SELECT ISS_SEVERITY_ID FROM DVM_ISS_SEVERITY WHERE ISS_SEVERITY_CODE = '",D3, "'), (SELECT data_stream_id from DVM_data_streams where data_stream_code = '",A3, "'), 'Y', '", SUBSTITUTE(I3, "'", "''"), "', '", SUBSTITUTE(K3, "'", "''"), "');")</f>
         <v>INSERT INTO DVM_ISS_TYPES (ISS_TYPE_NAME, ISS_TYPE_COMMENT_TEMPLATE, QC_OBJECT_ID, IND_FIELD_NAME, ISS_SEVERITY_ID, DATA_STREAM_ID, ISS_TYPE_ACTIVE_YN, ISS_TYPE_DESC, APP_LINK_TEMPLATE) VALUES ('Invalid Cruise Days at Sea', 'The Cruise ([CRUISE_NAME]) with Start Date ([FORMAT_CRUISE_START_DATE]) and End Date ([FORMAT_CRUISE_END_DATE]) and number of Legs ([NUM_LEGS]) has an invalid number ( &gt; 240) of Days at Sea ([CRUISE_DAS])', (SELECT QC_OBJECT_ID FROM DVM_QC_OBJECTS WHERE OBJECT_NAME = 'CCD_QC_CRUISE_V'), 'ERR_CRUISE_DAS_YN', (SELECT ISS_SEVERITY_ID FROM DVM_ISS_SEVERITY WHERE ISS_SEVERITY_CODE = 'ERROR'), (SELECT data_stream_id from DVM_data_streams where data_stream_code = 'CCD'), 'Y', 'Cruise is too long (DAS based on start and end dates) &gt; 240 days', 'f?p=[APP_ID]:220:[APP_SESSION]::NO::P220_CRUISE_ID,P220_CRUISE_ID_COPY:[CRUISE_ID],');</v>
       </c>
       <c r="O3" s="4"/>
@@ -1950,21 +1962,44 @@
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
     </row>
-    <row r="19" spans="1:24" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+    <row r="19" spans="1:24" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
+      <c r="N19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO DVM_ISS_TYPES (ISS_TYPE_NAME, ISS_TYPE_COMMENT_TEMPLATE, QC_OBJECT_ID, IND_FIELD_NAME, ISS_SEVERITY_ID, DATA_STREAM_ID, ISS_TYPE_ACTIVE_YN, ISS_TYPE_DESC, APP_LINK_TEMPLATE) VALUES ('Missing Leg Data Set', 'The Cruise ([CRUISE_NAME]) has a Cruise Leg ([LEG_NAME]) on the Vessel ([VESSEL_NAME]) with a Start Date ([FORMAT_LEG_START_DATE]) and End Date ([FORMAT_LEG_END_DATE]) that does not have at least one data set associated with it', (SELECT QC_OBJECT_ID FROM DVM_QC_OBJECTS WHERE OBJECT_NAME = 'CCD_QC_LEG_V'), 'MISS_DATA_SET_YN', (SELECT ISS_SEVERITY_ID FROM DVM_ISS_SEVERITY WHERE ISS_SEVERITY_CODE = 'WARN'), (SELECT data_stream_id from DVM_data_streams where data_stream_code = 'CCD'), 'Y', 'The Leg does not have any data sets defined for it', 'f?p=[APP_ID]:230:[APP_SESSION]::NO::P230_CRUISE_LEG_ID,P230_CRUISE_LEG_ID_COPY,P230_CRUISE_ID:[CRUISE_LEG_ID],,[CRUISE_ID]');</v>
+      </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
@@ -25056,7 +25091,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\Jesse.Abdul\Documents\Version Control\Git\centralized-cruise-database\docs\test cases\DVM_PKG\[test_QA_QC Validation Criteria.xlsx]List of Values'!#REF!</xm:f>
+            <xm:f>'C:\Users\jesse.abdul\Documents\Version Control\Git\centralized-cruise-database\docs\test cases\DVM_PKG\[test_QA_QC Validation Criteria.xlsx]List of Values'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D40:D56</xm:sqref>
         </x14:dataValidation>
@@ -25064,7 +25099,7 @@
           <x14:formula1>
             <xm:f>'[QC Validation Criteria Template.xlsx]List of Values'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D39 D57:D100</xm:sqref>
+          <xm:sqref>D57:D100 D2:D39</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>